<commit_message>
courses, staff, timeperiod completed git add .
</commit_message>
<xml_diff>
--- a/data/Student Data.xlsx
+++ b/data/Student Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="645" windowWidth="10215" windowHeight="4560"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="99">
   <si>
     <t>Admission Number(145261)</t>
   </si>
@@ -271,12 +271,6 @@
     <t>kajitsai7@gmail.com</t>
   </si>
   <si>
-    <t>Golla</t>
-  </si>
-  <si>
-    <t>golla.manish91@gmail.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mohanth </t>
   </si>
   <si>
@@ -293,6 +287,30 @@
   </si>
   <si>
     <t>nymishakandi@gmail.com</t>
+  </si>
+  <si>
+    <t>Shriya</t>
+  </si>
+  <si>
+    <t>Gali</t>
+  </si>
+  <si>
+    <t>shriyagali11@gmail.com</t>
+  </si>
+  <si>
+    <t>Shammi</t>
+  </si>
+  <si>
+    <t>shammi.akhil@gmail.com</t>
+  </si>
+  <si>
+    <t>Harsha Anirudh</t>
+  </si>
+  <si>
+    <t>GS</t>
+  </si>
+  <si>
+    <t>harsha.anirudh@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -642,27 +660,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I30" sqref="I30"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="17" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="2" customWidth="1"/>
+    <col min="3" max="17" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -980,7 +989,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>145207</v>
       </c>
@@ -1015,7 +1024,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>145225</v>
       </c>
@@ -1050,7 +1059,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>145258</v>
       </c>
@@ -1085,7 +1094,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>145209</v>
       </c>
@@ -1120,7 +1129,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>145241</v>
       </c>
@@ -1155,7 +1164,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>145212</v>
       </c>
@@ -1190,7 +1199,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>145228</v>
       </c>
@@ -1225,7 +1234,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>145215</v>
       </c>
@@ -1260,7 +1269,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>145230</v>
       </c>
@@ -1295,7 +1304,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>145232</v>
       </c>
@@ -1330,7 +1339,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>145234</v>
       </c>
@@ -1365,7 +1374,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>145211</v>
       </c>
@@ -1400,7 +1409,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>145210</v>
       </c>
@@ -1435,7 +1444,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>145223</v>
       </c>
@@ -1470,7 +1479,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>145213</v>
       </c>
@@ -1577,16 +1586,16 @@
     </row>
     <row r="27" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>145243</v>
+        <v>145264</v>
       </c>
       <c r="B27" s="3">
-        <v>160114733099</v>
+        <v>160114733316</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>13</v>
@@ -1598,13 +1607,13 @@
         <v>2</v>
       </c>
       <c r="H27" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I27" s="1">
-        <v>8019267367</v>
+        <v>9014994442</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>19</v>
@@ -1612,16 +1621,16 @@
     </row>
     <row r="28" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>145264</v>
+        <v>145237</v>
       </c>
       <c r="B28" s="3">
-        <v>160114733316</v>
+        <v>160114733072</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>13</v>
@@ -1633,13 +1642,13 @@
         <v>2</v>
       </c>
       <c r="H28" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I28" s="1">
-        <v>9014994442</v>
+        <v>9948033440</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>19</v>
@@ -1647,16 +1656,16 @@
     </row>
     <row r="29" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>145237</v>
+        <v>145248</v>
       </c>
       <c r="B29" s="3">
-        <v>160114733072</v>
+        <v>160114733078</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>13</v>
@@ -1671,12 +1680,82 @@
         <v>1</v>
       </c>
       <c r="I29" s="1">
-        <v>9948033440</v>
+        <v>8106996303</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K29" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>145239</v>
+      </c>
+      <c r="B30" s="3">
+        <v>160114733112</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="1">
+        <v>2</v>
+      </c>
+      <c r="H30" s="1">
+        <v>2</v>
+      </c>
+      <c r="I30" s="1">
+        <v>9848022338</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>145218</v>
+      </c>
+      <c r="B31" s="3">
+        <v>160114733095</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="1">
+        <v>2</v>
+      </c>
+      <c r="H31" s="1">
+        <v>2</v>
+      </c>
+      <c r="I31" s="1">
+        <v>9494949327</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K31" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>